<commit_message>
working python script with BH and SS
</commit_message>
<xml_diff>
--- a/states.xlsx
+++ b/states.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnrandolph/Desktop/Github/voting-power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE8994-4FEC-E54A-8381-AD9008F74FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330EBCD7-9D3F-C841-AB66-E3A5C95ABB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{41D7979D-D6FD-194B-8489-C32C243E0060}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Alabama</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>538_prob_red</t>
+  </si>
+  <si>
+    <t>Equal</t>
   </si>
 </sst>
 </file>
@@ -618,19 +621,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D65553-FC8A-F34B-BB8D-81E89D276CA3}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="11"/>
+    <col min="4" max="4" width="18.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="14" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -646,8 +650,11 @@
       <c r="E1" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +670,11 @@
       <c r="E2" s="11">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -680,8 +690,11 @@
       <c r="E3" s="11">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -697,8 +710,11 @@
       <c r="E4" s="11">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -714,8 +730,11 @@
       <c r="E5" s="11">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -731,8 +750,11 @@
       <c r="E6" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -748,8 +770,11 @@
       <c r="E7" s="11">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -765,8 +790,11 @@
       <c r="E8" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -782,8 +810,11 @@
       <c r="E9" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -799,8 +830,11 @@
       <c r="E10" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -816,8 +850,11 @@
       <c r="E11" s="11">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -833,8 +870,11 @@
       <c r="E12" s="11">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -850,8 +890,11 @@
       <c r="E13" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -867,8 +910,11 @@
       <c r="E14" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -884,8 +930,11 @@
       <c r="E15" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -901,8 +950,11 @@
       <c r="E16" s="11">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -918,8 +970,11 @@
       <c r="E17" s="11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -935,8 +990,11 @@
       <c r="E18" s="11">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -952,8 +1010,11 @@
       <c r="E19" s="11">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -969,8 +1030,11 @@
       <c r="E20" s="11">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -986,8 +1050,11 @@
       <c r="E21" s="11">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1003,8 +1070,11 @@
       <c r="E22" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1020,8 +1090,11 @@
       <c r="E23" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1037,8 +1110,11 @@
       <c r="E24" s="11">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1054,8 +1130,11 @@
       <c r="E25" s="11">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1071,8 +1150,11 @@
       <c r="E26" s="11">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1088,8 +1170,11 @@
       <c r="E27" s="11">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1105,8 +1190,11 @@
       <c r="E28" s="11">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1122,8 +1210,11 @@
       <c r="E29" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1139,8 +1230,11 @@
       <c r="E30" s="11">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1156,8 +1250,11 @@
       <c r="E31" s="11">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1173,8 +1270,11 @@
       <c r="E32" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1190,8 +1290,11 @@
       <c r="E33" s="11">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1207,8 +1310,11 @@
       <c r="E34" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1224,8 +1330,11 @@
       <c r="E35" s="11">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1241,8 +1350,11 @@
       <c r="E36" s="11">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1258,8 +1370,11 @@
       <c r="E37" s="11">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1275,8 +1390,11 @@
       <c r="E38" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1292,8 +1410,11 @@
       <c r="E39" s="11">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1309,8 +1430,11 @@
       <c r="E40" s="11">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1326,8 +1450,11 @@
       <c r="E41" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1343,8 +1470,11 @@
       <c r="E42" s="11">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1360,8 +1490,11 @@
       <c r="E43" s="11">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1377,8 +1510,11 @@
       <c r="E44" s="11">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1394,8 +1530,11 @@
       <c r="E45" s="11">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1411,8 +1550,11 @@
       <c r="E46" s="11">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1428,8 +1570,11 @@
       <c r="E47" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1445,8 +1590,11 @@
       <c r="E48" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1462,8 +1610,11 @@
       <c r="E49" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1479,8 +1630,11 @@
       <c r="E50" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1496,8 +1650,11 @@
       <c r="E51" s="11">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -1513,8 +1670,11 @@
       <c r="E52" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="4"/>
       <c r="C53" s="2"/>

</xml_diff>